<commit_message>
Rename variable for clarity
</commit_message>
<xml_diff>
--- a/efficiency.xlsx
+++ b/efficiency.xlsx
@@ -11,13 +11,17 @@
     <sheet name="Node" sheetId="2" r:id="rId5"/>
     <sheet name="Pod" sheetId="3" r:id="rId6"/>
     <sheet name="Namespace" sheetId="4" r:id="rId7"/>
+    <sheet name="Service" sheetId="5" r:id="rId8"/>
+    <sheet name="Deployment" sheetId="6" r:id="rId9"/>
+    <sheet name="Controller" sheetId="7" r:id="rId10"/>
+    <sheet name="controllerKind" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>Name</t>
   </si>
@@ -34,6 +38,9 @@
     <t>Window End</t>
   </si>
   <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
     <t>Total Efficiency</t>
   </si>
   <si>
@@ -43,13 +50,16 @@
     <t>ap-south-1</t>
   </si>
   <si>
-    <t>2024-07-21T07:00:00Z</t>
-  </si>
-  <si>
-    <t>2024-07-22T07:00:00Z</t>
-  </si>
-  <si>
-    <t>25.65</t>
+    <t>2024-07-22T03:00:00Z</t>
+  </si>
+  <si>
+    <t>2024-07-23T03:00:00Z</t>
+  </si>
+  <si>
+    <t>0.89</t>
+  </si>
+  <si>
+    <t>26.16</t>
   </si>
   <si>
     <t>Node</t>
@@ -58,130 +68,286 @@
     <t>ip-192-168-48-85.ap-south-1.compute.internal</t>
   </si>
   <si>
-    <t>33.30</t>
+    <t>0.77</t>
+  </si>
+  <si>
+    <t>34.63</t>
   </si>
   <si>
     <t>ip-192-168-95-236.ap-south-1.compute.internal</t>
   </si>
   <si>
-    <t>18.43</t>
+    <t>0.12</t>
+  </si>
+  <si>
+    <t>18.06</t>
+  </si>
+  <si>
+    <t>__idle__</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.68</t>
+  </si>
+  <si>
+    <t>0.00</t>
   </si>
   <si>
     <t>Pod</t>
   </si>
   <si>
+    <t>Namespace</t>
+  </si>
+  <si>
+    <t>coredns-5d5f56f475-5qfh2</t>
+  </si>
+  <si>
+    <t>kube-system</t>
+  </si>
+  <si>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>3.12</t>
+  </si>
+  <si>
+    <t>go-api-deployment-route1-dcbff4b58-wd8mh</t>
+  </si>
+  <si>
+    <t>route1</t>
+  </si>
+  <si>
+    <t>100.00</t>
+  </si>
+  <si>
+    <t>kubecost-cost-analyzer-685cd69b5-5v4jf</t>
+  </si>
+  <si>
+    <t>kubecost</t>
+  </si>
+  <si>
+    <t>0.66</t>
+  </si>
+  <si>
+    <t>167.51</t>
+  </si>
+  <si>
+    <t>aws-node-bc69s</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>17.62</t>
+  </si>
+  <si>
     <t>go-api-deployment-route2-85bb446767-hjnfv</t>
   </si>
   <si>
-    <t>100.00</t>
+    <t>route2</t>
   </si>
   <si>
     <t>kube-proxy-zx2rh</t>
   </si>
   <si>
-    <t>2.47</t>
+    <t>2.36</t>
+  </si>
+  <si>
+    <t>kubecost-forecasting-57947dfc5-dcl79</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>7.86</t>
+  </si>
+  <si>
+    <t>aws-node-v5rz9</t>
+  </si>
+  <si>
+    <t>16.98</t>
+  </si>
+  <si>
+    <t>coredns-5d5f56f475-kcdxs</t>
+  </si>
+  <si>
+    <t>3.11</t>
   </si>
   <si>
     <t>ebs-csi-controller-56c4dccdcb-b6zkl</t>
   </si>
   <si>
-    <t>9.86</t>
-  </si>
-  <si>
-    <t>go-api-deployment-route1-dcbff4b58-wd8mh</t>
+    <t>10.54</t>
+  </si>
+  <si>
+    <t>ebs-csi-controller-56c4dccdcb-rm8g8</t>
+  </si>
+  <si>
+    <t>15.41</t>
+  </si>
+  <si>
+    <t>ebs-csi-node-tbz4n</t>
+  </si>
+  <si>
+    <t>14.70</t>
+  </si>
+  <si>
+    <t>go-api-deployment-route1-dcbff4b58-d2br2</t>
+  </si>
+  <si>
+    <t>kubecost-grafana-585668695-ww4cf</t>
   </si>
   <si>
     <t>ebs-csi-node-6qf47</t>
   </si>
   <si>
-    <t>9.21</t>
-  </si>
-  <si>
-    <t>ebs-csi-node-tbz4n</t>
-  </si>
-  <si>
-    <t>14.58</t>
+    <t>11.52</t>
+  </si>
+  <si>
+    <t>go-api-deployment-route2-85bb446767-lqq5v</t>
   </si>
   <si>
     <t>kube-proxy-ngxfx</t>
   </si>
   <si>
-    <t>2.22</t>
-  </si>
-  <si>
-    <t>kubecost-grafana-585668695-ww4cf</t>
+    <t>2.17</t>
   </si>
   <si>
     <t>kubecost-prometheus-server-78f6878b66-zff6l</t>
   </si>
   <si>
-    <t>coredns-5d5f56f475-5qfh2</t>
-  </si>
-  <si>
-    <t>2.94</t>
-  </si>
-  <si>
-    <t>coredns-5d5f56f475-kcdxs</t>
-  </si>
-  <si>
-    <t>2.95</t>
-  </si>
-  <si>
-    <t>ebs-csi-controller-56c4dccdcb-rm8g8</t>
-  </si>
-  <si>
-    <t>16.50</t>
-  </si>
-  <si>
-    <t>kubecost-cost-analyzer-685cd69b5-5v4jf</t>
-  </si>
-  <si>
-    <t>165.27</t>
-  </si>
-  <si>
-    <t>go-api-deployment-route1-dcbff4b58-d2br2</t>
-  </si>
-  <si>
-    <t>go-api-deployment-route2-85bb446767-lqq5v</t>
-  </si>
-  <si>
-    <t>kubecost-forecasting-57947dfc5-dcl79</t>
-  </si>
-  <si>
-    <t>7.85</t>
-  </si>
-  <si>
-    <t>aws-node-bc69s</t>
-  </si>
-  <si>
-    <t>18.11</t>
-  </si>
-  <si>
-    <t>aws-node-v5rz9</t>
-  </si>
-  <si>
-    <t>17.05</t>
-  </si>
-  <si>
-    <t>Namespace</t>
-  </si>
-  <si>
-    <t>route1</t>
-  </si>
-  <si>
-    <t>route2</t>
-  </si>
-  <si>
-    <t>kube-system</t>
-  </si>
-  <si>
-    <t>9.14</t>
-  </si>
-  <si>
-    <t>kubecost</t>
-  </si>
-  <si>
-    <t>69.37</t>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>70.02</t>
+  </si>
+  <si>
+    <t>0.18</t>
+  </si>
+  <si>
+    <t>9.44</t>
+  </si>
+  <si>
+    <t>"kubecost-prometheus-server"</t>
+  </si>
+  <si>
+    <t>__unallocated__</t>
+  </si>
+  <si>
+    <t>0.13</t>
+  </si>
+  <si>
+    <t>11.90</t>
+  </si>
+  <si>
+    <t>"kubecost-aggregator"</t>
+  </si>
+  <si>
+    <t>0.27</t>
+  </si>
+  <si>
+    <t>155.01</t>
+  </si>
+  <si>
+    <t>"kubecost-grafana"</t>
+  </si>
+  <si>
+    <t>"kube-dns"</t>
+  </si>
+  <si>
+    <t>"kubecost-cloud-cost"</t>
+  </si>
+  <si>
+    <t>0.24</t>
+  </si>
+  <si>
+    <t>181.47</t>
+  </si>
+  <si>
+    <t>"kubecost-cost-analyzer"</t>
+  </si>
+  <si>
+    <t>0.15</t>
+  </si>
+  <si>
+    <t>166.91</t>
+  </si>
+  <si>
+    <t>"kubecost-forecasting"</t>
+  </si>
+  <si>
+    <t>"go-route1-service"</t>
+  </si>
+  <si>
+    <t>"go-route2-service"</t>
+  </si>
+  <si>
+    <t>coredns</t>
+  </si>
+  <si>
+    <t>ebs-csi-controller</t>
+  </si>
+  <si>
+    <t>0.04</t>
+  </si>
+  <si>
+    <t>12.97</t>
+  </si>
+  <si>
+    <t>kubecost-prometheus-server</t>
+  </si>
+  <si>
+    <t>go-api-deployment-route2</t>
+  </si>
+  <si>
+    <t>kubecost-cost-analyzer</t>
+  </si>
+  <si>
+    <t>kubecost-forecasting</t>
+  </si>
+  <si>
+    <t>kubecost-grafana</t>
+  </si>
+  <si>
+    <t>go-api-deployment-route1</t>
+  </si>
+  <si>
+    <t>kube-proxy</t>
+  </si>
+  <si>
+    <t>2.26</t>
+  </si>
+  <si>
+    <t>aws-node</t>
+  </si>
+  <si>
+    <t>17.30</t>
+  </si>
+  <si>
+    <t>ebs-csi-node</t>
+  </si>
+  <si>
+    <t>13.11</t>
+  </si>
+  <si>
+    <t>daemonset</t>
+  </si>
+  <si>
+    <t>0.09</t>
+  </si>
+  <si>
+    <t>13.20</t>
+  </si>
+  <si>
+    <t>deployment</t>
+  </si>
+  <si>
+    <t>0.80</t>
+  </si>
+  <si>
+    <t>31.71</t>
   </si>
 </sst>
 </file>
@@ -510,25 +676,31 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -547,7 +719,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -561,45 +733,77 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -618,379 +822,519 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
         <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>43</v>
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>45</v>
+        <v>10</v>
+      </c>
+      <c r="G18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
         <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>47</v>
+        <v>10</v>
+      </c>
+      <c r="G19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1009,7 +1353,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1023,85 +1367,1052 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>65</v>
+      </c>
+      <c r="G2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Add logger to the whole script
</commit_message>
<xml_diff>
--- a/efficiency.xlsx
+++ b/efficiency.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>Name</t>
   </si>
@@ -50,28 +50,40 @@
     <t>ap-south-1</t>
   </si>
   <si>
-    <t>2024-07-22T03:00:00Z</t>
-  </si>
-  <si>
-    <t>2024-07-23T03:00:00Z</t>
+    <t>2024-07-22T07:00:00Z</t>
+  </si>
+  <si>
+    <t>2024-07-23T07:00:00Z</t>
   </si>
   <si>
     <t>0.89</t>
   </si>
   <si>
-    <t>26.16</t>
+    <t>26.50</t>
   </si>
   <si>
     <t>Node</t>
   </si>
   <si>
+    <t>__idle__</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.68</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
     <t>ip-192-168-48-85.ap-south-1.compute.internal</t>
   </si>
   <si>
     <t>0.77</t>
   </si>
   <si>
-    <t>34.63</t>
+    <t>35.19</t>
   </si>
   <si>
     <t>ip-192-168-95-236.ap-south-1.compute.internal</t>
@@ -80,19 +92,7 @@
     <t>0.12</t>
   </si>
   <si>
-    <t>18.06</t>
-  </si>
-  <si>
-    <t>__idle__</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>0.68</t>
-  </si>
-  <si>
-    <t>0.00</t>
+    <t>18.17</t>
   </si>
   <si>
     <t>Pod</t>
@@ -101,25 +101,73 @@
     <t>Namespace</t>
   </si>
   <si>
+    <t>go-api-deployment-route1-dcbff4b58-wd8mh</t>
+  </si>
+  <si>
+    <t>route1</t>
+  </si>
+  <si>
+    <t>100.00</t>
+  </si>
+  <si>
+    <t>aws-node-bc69s</t>
+  </si>
+  <si>
+    <t>kube-system</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>18.07</t>
+  </si>
+  <si>
     <t>coredns-5d5f56f475-5qfh2</t>
   </si>
   <si>
-    <t>kube-system</t>
-  </si>
-  <si>
     <t>0.02</t>
   </si>
   <si>
+    <t>3.14</t>
+  </si>
+  <si>
+    <t>ebs-csi-node-6qf47</t>
+  </si>
+  <si>
+    <t>12.13</t>
+  </si>
+  <si>
+    <t>ebs-csi-node-tbz4n</t>
+  </si>
+  <si>
+    <t>14.72</t>
+  </si>
+  <si>
+    <t>ebs-csi-controller-56c4dccdcb-rm8g8</t>
+  </si>
+  <si>
+    <t>15.30</t>
+  </si>
+  <si>
+    <t>go-api-deployment-route1-dcbff4b58-d2br2</t>
+  </si>
+  <si>
+    <t>kube-proxy-zx2rh</t>
+  </si>
+  <si>
+    <t>2.47</t>
+  </si>
+  <si>
+    <t>coredns-5d5f56f475-kcdxs</t>
+  </si>
+  <si>
     <t>3.12</t>
   </si>
   <si>
-    <t>go-api-deployment-route1-dcbff4b58-wd8mh</t>
-  </si>
-  <si>
-    <t>route1</t>
-  </si>
-  <si>
-    <t>100.00</t>
+    <t>ebs-csi-controller-56c4dccdcb-b6zkl</t>
+  </si>
+  <si>
+    <t>10.68</t>
   </si>
   <si>
     <t>kubecost-cost-analyzer-685cd69b5-5v4jf</t>
@@ -131,103 +179,55 @@
     <t>0.66</t>
   </si>
   <si>
-    <t>167.51</t>
-  </si>
-  <si>
-    <t>aws-node-bc69s</t>
-  </si>
-  <si>
-    <t>0.01</t>
-  </si>
-  <si>
-    <t>17.62</t>
+    <t>169.50</t>
+  </si>
+  <si>
+    <t>kubecost-grafana-585668695-ww4cf</t>
+  </si>
+  <si>
+    <t>kube-proxy-ngxfx</t>
+  </si>
+  <si>
+    <t>2.21</t>
+  </si>
+  <si>
+    <t>kubecost-forecasting-57947dfc5-dcl79</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>7.86</t>
+  </si>
+  <si>
+    <t>kubecost-prometheus-server-78f6878b66-zff6l</t>
+  </si>
+  <si>
+    <t>route2</t>
+  </si>
+  <si>
+    <t>aws-node-v5rz9</t>
+  </si>
+  <si>
+    <t>17.30</t>
   </si>
   <si>
     <t>go-api-deployment-route2-85bb446767-hjnfv</t>
   </si>
   <si>
-    <t>route2</t>
-  </si>
-  <si>
-    <t>kube-proxy-zx2rh</t>
-  </si>
-  <si>
-    <t>2.36</t>
-  </si>
-  <si>
-    <t>kubecost-forecasting-57947dfc5-dcl79</t>
-  </si>
-  <si>
-    <t>0.05</t>
-  </si>
-  <si>
-    <t>7.86</t>
-  </si>
-  <si>
-    <t>aws-node-v5rz9</t>
-  </si>
-  <si>
-    <t>16.98</t>
-  </si>
-  <si>
-    <t>coredns-5d5f56f475-kcdxs</t>
-  </si>
-  <si>
-    <t>3.11</t>
-  </si>
-  <si>
-    <t>ebs-csi-controller-56c4dccdcb-b6zkl</t>
-  </si>
-  <si>
-    <t>10.54</t>
-  </si>
-  <si>
-    <t>ebs-csi-controller-56c4dccdcb-rm8g8</t>
-  </si>
-  <si>
-    <t>15.41</t>
-  </si>
-  <si>
-    <t>ebs-csi-node-tbz4n</t>
-  </si>
-  <si>
-    <t>14.70</t>
-  </si>
-  <si>
-    <t>go-api-deployment-route1-dcbff4b58-d2br2</t>
-  </si>
-  <si>
-    <t>kubecost-grafana-585668695-ww4cf</t>
-  </si>
-  <si>
-    <t>ebs-csi-node-6qf47</t>
-  </si>
-  <si>
-    <t>11.52</t>
-  </si>
-  <si>
     <t>go-api-deployment-route2-85bb446767-lqq5v</t>
   </si>
   <si>
-    <t>kube-proxy-ngxfx</t>
-  </si>
-  <si>
-    <t>2.17</t>
-  </si>
-  <si>
-    <t>kubecost-prometheus-server-78f6878b66-zff6l</t>
+    <t>0.18</t>
+  </si>
+  <si>
+    <t>9.56</t>
   </si>
   <si>
     <t>0.72</t>
   </si>
   <si>
-    <t>70.02</t>
-  </si>
-  <si>
-    <t>0.18</t>
-  </si>
-  <si>
-    <t>9.44</t>
+    <t>70.88</t>
   </si>
   <si>
     <t>"kubecost-prometheus-server"</t>
@@ -239,49 +239,61 @@
     <t>0.13</t>
   </si>
   <si>
-    <t>11.90</t>
+    <t>12.07</t>
+  </si>
+  <si>
+    <t>"kube-dns"</t>
+  </si>
+  <si>
+    <t>3.13</t>
   </si>
   <si>
     <t>"kubecost-aggregator"</t>
   </si>
   <si>
-    <t>0.27</t>
-  </si>
-  <si>
-    <t>155.01</t>
+    <t>0.39</t>
+  </si>
+  <si>
+    <t>163.95</t>
+  </si>
+  <si>
+    <t>"kubecost-cloud-cost"</t>
+  </si>
+  <si>
+    <t>185.07</t>
+  </si>
+  <si>
+    <t>"kubecost-cost-analyzer"</t>
+  </si>
+  <si>
+    <t>0.09</t>
+  </si>
+  <si>
+    <t>162.47</t>
   </si>
   <si>
     <t>"kubecost-grafana"</t>
   </si>
   <si>
-    <t>"kube-dns"</t>
-  </si>
-  <si>
-    <t>"kubecost-cloud-cost"</t>
-  </si>
-  <si>
-    <t>0.24</t>
-  </si>
-  <si>
-    <t>181.47</t>
-  </si>
-  <si>
-    <t>"kubecost-cost-analyzer"</t>
-  </si>
-  <si>
-    <t>0.15</t>
-  </si>
-  <si>
-    <t>166.91</t>
+    <t>"go-route1-service"</t>
+  </si>
+  <si>
+    <t>"go-route2-service"</t>
   </si>
   <si>
     <t>"kubecost-forecasting"</t>
   </si>
   <si>
-    <t>"go-route1-service"</t>
-  </si>
-  <si>
-    <t>"go-route2-service"</t>
+    <t>go-api-deployment-route1</t>
+  </si>
+  <si>
+    <t>kubecost-cost-analyzer</t>
+  </si>
+  <si>
+    <t>kubecost-grafana</t>
+  </si>
+  <si>
+    <t>kubecost-prometheus-server</t>
   </si>
   <si>
     <t>coredns</t>
@@ -293,52 +305,37 @@
     <t>0.04</t>
   </si>
   <si>
-    <t>12.97</t>
-  </si>
-  <si>
-    <t>kubecost-prometheus-server</t>
+    <t>12.99</t>
   </si>
   <si>
     <t>go-api-deployment-route2</t>
   </si>
   <si>
-    <t>kubecost-cost-analyzer</t>
-  </si>
-  <si>
     <t>kubecost-forecasting</t>
   </si>
   <si>
-    <t>kubecost-grafana</t>
-  </si>
-  <si>
-    <t>go-api-deployment-route1</t>
+    <t>aws-node</t>
+  </si>
+  <si>
+    <t>17.69</t>
+  </si>
+  <si>
+    <t>ebs-csi-node</t>
+  </si>
+  <si>
+    <t>13.43</t>
   </si>
   <si>
     <t>kube-proxy</t>
   </si>
   <si>
-    <t>2.26</t>
-  </si>
-  <si>
-    <t>aws-node</t>
-  </si>
-  <si>
-    <t>17.30</t>
-  </si>
-  <si>
-    <t>ebs-csi-node</t>
-  </si>
-  <si>
-    <t>13.11</t>
+    <t>2.34</t>
   </si>
   <si>
     <t>daemonset</t>
   </si>
   <si>
-    <t>0.09</t>
-  </si>
-  <si>
-    <t>13.20</t>
+    <t>13.55</t>
   </si>
   <si>
     <t>deployment</t>
@@ -347,7 +344,7 @@
     <t>0.80</t>
   </si>
   <si>
-    <t>31.71</t>
+    <t>32.04</t>
   </si>
 </sst>
 </file>
@@ -745,7 +742,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -754,18 +751,18 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -777,21 +774,21 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -863,33 +860,33 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
         <v>28</v>
-      </c>
-      <c r="H2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
         <v>31</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
       </c>
       <c r="H3" t="s">
         <v>32</v>
@@ -906,59 +903,59 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
         <v>34</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>35</v>
-      </c>
-      <c r="H4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
         <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -967,24 +964,24 @@
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -993,24 +990,24 @@
         <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
@@ -1019,24 +1016,24 @@
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -1045,24 +1042,24 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -1071,24 +1068,24 @@
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -1097,24 +1094,24 @@
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
@@ -1123,24 +1120,24 @@
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="H12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
@@ -1149,24 +1146,24 @@
         <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="H13" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
@@ -1175,50 +1172,50 @@
         <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="H14" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" t="s">
         <v>58</v>
-      </c>
-      <c r="B15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
@@ -1227,24 +1224,24 @@
         <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H16" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
@@ -1253,10 +1250,10 @@
         <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="H17" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18">
@@ -1270,7 +1267,7 @@
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
@@ -1279,24 +1276,24 @@
         <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="H18" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s">
         <v>9</v>
@@ -1305,10 +1302,10 @@
         <v>10</v>
       </c>
       <c r="G19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" t="s">
         <v>28</v>
-      </c>
-      <c r="H19" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="20">
@@ -1322,7 +1319,7 @@
         <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
         <v>9</v>
@@ -1331,10 +1328,10 @@
         <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H20" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1373,13 +1370,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -1388,18 +1385,18 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -1411,18 +1408,18 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -1434,21 +1431,21 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -1457,18 +1454,18 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -1480,10 +1477,10 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1528,7 +1525,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -1537,21 +1534,21 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -1560,21 +1557,21 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -1583,21 +1580,21 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -1606,21 +1603,21 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -1629,21 +1626,21 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1652,21 +1649,21 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -1675,21 +1672,21 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -1698,21 +1695,21 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -1721,21 +1718,21 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
@@ -1744,21 +1741,21 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="G11" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -1767,10 +1764,10 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="G12" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1809,14 +1806,11 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
@@ -1824,15 +1818,15 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -1847,21 +1841,21 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -1870,21 +1864,21 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -1893,21 +1887,21 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -1916,21 +1910,21 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1939,21 +1933,21 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -1962,19 +1956,22 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>93</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
@@ -1982,10 +1979,10 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
@@ -1996,7 +1993,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -2005,10 +2002,10 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2047,13 +2044,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -2062,21 +2059,21 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -2085,21 +2082,21 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -2108,21 +2105,21 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -2131,15 +2128,15 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -2154,21 +2151,21 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>98</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -2177,21 +2174,21 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -2200,21 +2197,21 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -2223,21 +2220,21 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -2246,21 +2243,21 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
         <v>28</v>
-      </c>
-      <c r="G10" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
@@ -2269,21 +2266,21 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -2292,21 +2289,21 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="G12" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
@@ -2315,10 +2312,10 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2357,10 +2354,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -2369,10 +2366,10 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
@@ -2389,30 +2386,30 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" t="s">
         <v>104</v>
-      </c>
-      <c r="F3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>106</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>107</v>
-      </c>
-      <c r="F4" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>